<commit_message>
updated public function registerEvents in DTRExport
</commit_message>
<xml_diff>
--- a/resources/templates/template.xlsx
+++ b/resources/templates/template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\LARIS DATA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\NIA\resources\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{612277A8-3F25-4C29-BC5D-C061BCB93295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39FFFB2E-7EAC-4B18-A168-B5483EB62902}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="24">
   <si>
     <t>D A I L Y    T I M E    R E C O R D</t>
   </si>
@@ -116,60 +116,13 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Cambria"/>
+        <family val="1"/>
       </rPr>
       <t xml:space="preserve">Falsification of time records will render the offending officers or employee liable to summary removal from the service and criminal prosecution. </t>
     </r>
   </si>
   <si>
-    <t>01</t>
-  </si>
-  <si>
-    <t>02</t>
-  </si>
-  <si>
-    <t>03</t>
-  </si>
-  <si>
-    <t>04</t>
-  </si>
-  <si>
-    <t>05</t>
-  </si>
-  <si>
-    <t>06</t>
-  </si>
-  <si>
-    <t>07</t>
-  </si>
-  <si>
-    <t>08</t>
-  </si>
-  <si>
-    <t>09</t>
-  </si>
-  <si>
     <t>N/A</t>
-  </si>
-  <si>
-    <t>Sunday</t>
-  </si>
-  <si>
-    <t>Monday</t>
-  </si>
-  <si>
-    <t>Tuesday</t>
-  </si>
-  <si>
-    <t>Wednesday</t>
-  </si>
-  <si>
-    <t>Thursday</t>
-  </si>
-  <si>
-    <t>Friday</t>
-  </si>
-  <si>
-    <t>Saturday</t>
   </si>
 </sst>
 </file>
@@ -191,56 +144,66 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
+      <family val="1"/>
     </font>
     <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
+      <family val="1"/>
     </font>
     <font>
       <i/>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
       <sz val="24"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
       <name val="Cambria"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
       <name val="Cambria"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
@@ -248,6 +211,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="9"/>
@@ -792,12 +756,27 @@
     <xf numFmtId="18" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="18" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -806,21 +785,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2076,7 +2040,7 @@
   <dimension ref="A7:U46"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="67" zoomScaleNormal="60" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2197,34 +2161,28 @@
     <row r="12" spans="1:19" s="8" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="14"/>
       <c r="B12" s="30"/>
-      <c r="C12" s="70" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" s="70"/>
+      <c r="C12" s="71"/>
+      <c r="D12" s="71"/>
       <c r="E12" s="31"/>
       <c r="F12" s="31"/>
       <c r="G12" s="31"/>
       <c r="H12" s="31"/>
       <c r="I12" s="31"/>
-      <c r="J12" s="67"/>
-      <c r="K12" s="67"/>
+      <c r="J12" s="72"/>
+      <c r="K12" s="72"/>
       <c r="L12" s="32"/>
       <c r="M12" s="32"/>
       <c r="N12" s="32"/>
       <c r="O12" s="32"/>
-      <c r="P12" s="68"/>
-      <c r="Q12" s="69"/>
-      <c r="R12" s="33" t="s">
-        <v>23</v>
-      </c>
+      <c r="P12" s="73"/>
+      <c r="Q12" s="74"/>
+      <c r="R12" s="33"/>
     </row>
     <row r="13" spans="1:19" s="8" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14"/>
       <c r="B13" s="25"/>
-      <c r="C13" s="71" t="s">
-        <v>34</v>
-      </c>
-      <c r="D13" s="71"/>
+      <c r="C13" s="67"/>
+      <c r="D13" s="67"/>
       <c r="E13" s="18"/>
       <c r="F13" s="18"/>
       <c r="G13" s="18"/>
@@ -2238,17 +2196,13 @@
       <c r="O13" s="19"/>
       <c r="P13" s="46"/>
       <c r="Q13" s="47"/>
-      <c r="R13" s="20" t="s">
-        <v>24</v>
-      </c>
+      <c r="R13" s="20"/>
     </row>
     <row r="14" spans="1:19" s="8" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="14"/>
       <c r="B14" s="25"/>
-      <c r="C14" s="71" t="s">
-        <v>35</v>
-      </c>
-      <c r="D14" s="71"/>
+      <c r="C14" s="67"/>
+      <c r="D14" s="67"/>
       <c r="E14" s="18"/>
       <c r="F14" s="18"/>
       <c r="G14" s="18"/>
@@ -2262,17 +2216,13 @@
       <c r="O14" s="19"/>
       <c r="P14" s="46"/>
       <c r="Q14" s="47"/>
-      <c r="R14" s="20" t="s">
-        <v>25</v>
-      </c>
+      <c r="R14" s="20"/>
     </row>
     <row r="15" spans="1:19" s="8" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14"/>
       <c r="B15" s="25"/>
-      <c r="C15" s="71" t="s">
-        <v>36</v>
-      </c>
-      <c r="D15" s="71"/>
+      <c r="C15" s="67"/>
+      <c r="D15" s="67"/>
       <c r="E15" s="18"/>
       <c r="F15" s="18"/>
       <c r="G15" s="18"/>
@@ -2286,17 +2236,13 @@
       <c r="O15" s="19"/>
       <c r="P15" s="46"/>
       <c r="Q15" s="47"/>
-      <c r="R15" s="20" t="s">
-        <v>26</v>
-      </c>
+      <c r="R15" s="20"/>
     </row>
     <row r="16" spans="1:19" s="8" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="14"/>
       <c r="B16" s="25"/>
-      <c r="C16" s="71" t="s">
-        <v>37</v>
-      </c>
-      <c r="D16" s="71"/>
+      <c r="C16" s="67"/>
+      <c r="D16" s="67"/>
       <c r="E16" s="18"/>
       <c r="F16" s="18"/>
       <c r="G16" s="18"/>
@@ -2310,17 +2256,13 @@
       <c r="O16" s="19"/>
       <c r="P16" s="46"/>
       <c r="Q16" s="47"/>
-      <c r="R16" s="20" t="s">
-        <v>27</v>
-      </c>
+      <c r="R16" s="20"/>
     </row>
     <row r="17" spans="1:21" s="8" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14"/>
       <c r="B17" s="25"/>
-      <c r="C17" s="71" t="s">
-        <v>38</v>
-      </c>
-      <c r="D17" s="71"/>
+      <c r="C17" s="67"/>
+      <c r="D17" s="67"/>
       <c r="E17" s="18"/>
       <c r="F17" s="18"/>
       <c r="G17" s="18"/>
@@ -2334,17 +2276,13 @@
       <c r="O17" s="19"/>
       <c r="P17" s="46"/>
       <c r="Q17" s="47"/>
-      <c r="R17" s="20" t="s">
-        <v>28</v>
-      </c>
+      <c r="R17" s="20"/>
     </row>
     <row r="18" spans="1:21" s="8" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="14"/>
       <c r="B18" s="34"/>
-      <c r="C18" s="72" t="s">
-        <v>39</v>
-      </c>
-      <c r="D18" s="72"/>
+      <c r="C18" s="68"/>
+      <c r="D18" s="68"/>
       <c r="E18" s="35"/>
       <c r="F18" s="35"/>
       <c r="G18" s="35"/>
@@ -2356,19 +2294,15 @@
       <c r="M18" s="36"/>
       <c r="N18" s="36"/>
       <c r="O18" s="36"/>
-      <c r="P18" s="65"/>
-      <c r="Q18" s="66"/>
-      <c r="R18" s="37" t="s">
-        <v>29</v>
-      </c>
+      <c r="P18" s="69"/>
+      <c r="Q18" s="70"/>
+      <c r="R18" s="37"/>
     </row>
     <row r="19" spans="1:21" s="8" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="14"/>
       <c r="B19" s="34"/>
-      <c r="C19" s="72" t="s">
-        <v>33</v>
-      </c>
-      <c r="D19" s="72"/>
+      <c r="C19" s="68"/>
+      <c r="D19" s="68"/>
       <c r="E19" s="35"/>
       <c r="F19" s="35"/>
       <c r="G19" s="35"/>
@@ -2380,19 +2314,15 @@
       <c r="M19" s="36"/>
       <c r="N19" s="36"/>
       <c r="O19" s="36"/>
-      <c r="P19" s="65"/>
-      <c r="Q19" s="66"/>
-      <c r="R19" s="37" t="s">
-        <v>30</v>
-      </c>
+      <c r="P19" s="69"/>
+      <c r="Q19" s="70"/>
+      <c r="R19" s="37"/>
     </row>
     <row r="20" spans="1:21" s="8" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="14"/>
       <c r="B20" s="25"/>
-      <c r="C20" s="71" t="s">
-        <v>34</v>
-      </c>
-      <c r="D20" s="71"/>
+      <c r="C20" s="67"/>
+      <c r="D20" s="67"/>
       <c r="E20" s="18"/>
       <c r="F20" s="18"/>
       <c r="G20" s="18"/>
@@ -2406,17 +2336,13 @@
       <c r="O20" s="19"/>
       <c r="P20" s="46"/>
       <c r="Q20" s="47"/>
-      <c r="R20" s="20" t="s">
-        <v>31</v>
-      </c>
+      <c r="R20" s="20"/>
     </row>
     <row r="21" spans="1:21" s="8" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="14"/>
       <c r="B21" s="25"/>
-      <c r="C21" s="71" t="s">
-        <v>35</v>
-      </c>
-      <c r="D21" s="71"/>
+      <c r="C21" s="67"/>
+      <c r="D21" s="67"/>
       <c r="E21" s="18"/>
       <c r="F21" s="18"/>
       <c r="G21" s="18"/>
@@ -2430,17 +2356,13 @@
       <c r="O21" s="19"/>
       <c r="P21" s="46"/>
       <c r="Q21" s="47"/>
-      <c r="R21" s="20">
-        <v>10</v>
-      </c>
+      <c r="R21" s="20"/>
     </row>
     <row r="22" spans="1:21" s="8" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="14"/>
       <c r="B22" s="25"/>
-      <c r="C22" s="71" t="s">
-        <v>36</v>
-      </c>
-      <c r="D22" s="71"/>
+      <c r="C22" s="67"/>
+      <c r="D22" s="67"/>
       <c r="E22" s="18"/>
       <c r="F22" s="18"/>
       <c r="G22" s="18"/>
@@ -2454,17 +2376,13 @@
       <c r="O22" s="19"/>
       <c r="P22" s="46"/>
       <c r="Q22" s="47"/>
-      <c r="R22" s="20">
-        <v>11</v>
-      </c>
+      <c r="R22" s="20"/>
     </row>
     <row r="23" spans="1:21" s="8" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="14"/>
       <c r="B23" s="25"/>
-      <c r="C23" s="71" t="s">
-        <v>37</v>
-      </c>
-      <c r="D23" s="71"/>
+      <c r="C23" s="67"/>
+      <c r="D23" s="67"/>
       <c r="E23" s="18"/>
       <c r="F23" s="18"/>
       <c r="G23" s="18"/>
@@ -2478,17 +2396,13 @@
       <c r="O23" s="19"/>
       <c r="P23" s="46"/>
       <c r="Q23" s="47"/>
-      <c r="R23" s="20">
-        <v>12</v>
-      </c>
+      <c r="R23" s="20"/>
     </row>
     <row r="24" spans="1:21" s="8" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="14"/>
       <c r="B24" s="25"/>
-      <c r="C24" s="71" t="s">
-        <v>38</v>
-      </c>
-      <c r="D24" s="71"/>
+      <c r="C24" s="67"/>
+      <c r="D24" s="67"/>
       <c r="E24" s="18"/>
       <c r="F24" s="18"/>
       <c r="G24" s="18"/>
@@ -2502,17 +2416,13 @@
       <c r="O24" s="19"/>
       <c r="P24" s="46"/>
       <c r="Q24" s="47"/>
-      <c r="R24" s="20">
-        <v>13</v>
-      </c>
+      <c r="R24" s="20"/>
     </row>
     <row r="25" spans="1:21" s="8" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="14"/>
       <c r="B25" s="34"/>
-      <c r="C25" s="72" t="s">
-        <v>39</v>
-      </c>
-      <c r="D25" s="72"/>
+      <c r="C25" s="68"/>
+      <c r="D25" s="68"/>
       <c r="E25" s="35"/>
       <c r="F25" s="35"/>
       <c r="G25" s="35"/>
@@ -2524,19 +2434,15 @@
       <c r="M25" s="36"/>
       <c r="N25" s="36"/>
       <c r="O25" s="36"/>
-      <c r="P25" s="65"/>
-      <c r="Q25" s="66"/>
-      <c r="R25" s="37">
-        <v>14</v>
-      </c>
+      <c r="P25" s="69"/>
+      <c r="Q25" s="70"/>
+      <c r="R25" s="37"/>
     </row>
     <row r="26" spans="1:21" s="8" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="14"/>
       <c r="B26" s="34"/>
-      <c r="C26" s="72" t="s">
-        <v>33</v>
-      </c>
-      <c r="D26" s="72"/>
+      <c r="C26" s="68"/>
+      <c r="D26" s="68"/>
       <c r="E26" s="35"/>
       <c r="F26" s="35"/>
       <c r="G26" s="35"/>
@@ -2548,17 +2454,15 @@
       <c r="M26" s="36"/>
       <c r="N26" s="36"/>
       <c r="O26" s="36"/>
-      <c r="P26" s="65"/>
-      <c r="Q26" s="66"/>
-      <c r="R26" s="37">
-        <v>15</v>
-      </c>
+      <c r="P26" s="69"/>
+      <c r="Q26" s="70"/>
+      <c r="R26" s="37"/>
     </row>
     <row r="27" spans="1:21" s="8" customFormat="1" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="14"/>
       <c r="B27" s="26"/>
-      <c r="C27" s="73"/>
-      <c r="D27" s="74"/>
+      <c r="C27" s="65"/>
+      <c r="D27" s="66"/>
       <c r="E27" s="21"/>
       <c r="F27" s="21"/>
       <c r="G27" s="21"/>
@@ -2658,7 +2562,7 @@
       <c r="I34" s="27"/>
       <c r="J34" s="3"/>
       <c r="K34" s="38" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="L34" s="38"/>
       <c r="M34" s="38"/>

</xml_diff>